<commit_message>
Ajout de la fonction "favorite".
</commit_message>
<xml_diff>
--- a/UserStory.xlsx
+++ b/UserStory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
   <si>
     <t>User Story</t>
   </si>
@@ -758,14 +758,14 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -790,7 +790,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -831,43 +831,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1264,24 +1228,24 @@
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="39"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -2194,6 +2158,63 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="73">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H7:K7"/>
@@ -2210,63 +2231,6 @@
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2277,8 +2241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2625,9 +2589,11 @@
         <v>74</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="H9" s="9"/>
       <c r="I9" s="18"/>
       <c r="J9" s="8">
@@ -2667,9 +2633,11 @@
         <v>73</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="H10" s="9"/>
       <c r="I10" s="18"/>
       <c r="J10" s="8">
@@ -2748,7 +2716,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D12" s="9">
         <v>500</v>
@@ -2757,7 +2725,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>90</v>
@@ -2794,7 +2762,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D13" s="9">
         <v>700</v>
@@ -2838,7 +2806,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D14" s="9">
         <v>700</v>
@@ -2884,7 +2852,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D15" s="9">
         <v>800</v>
@@ -2893,9 +2861,11 @@
         <v>84</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="9"/>
+        <v>70</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="H15" s="9"/>
       <c r="I15" s="18"/>
       <c r="J15" s="8">
@@ -2926,7 +2896,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D16" s="9">
         <v>500</v>
@@ -2937,7 +2907,9 @@
       <c r="F16" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="H16" s="9"/>
       <c r="I16" s="18"/>
       <c r="J16" s="8">
@@ -2970,7 +2942,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17" s="9">
         <v>100</v>
@@ -2979,9 +2951,11 @@
         <v>86</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="9"/>
+        <v>70</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="H17" s="9"/>
       <c r="I17" s="18"/>
       <c r="J17" s="8">
@@ -3014,7 +2988,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="8">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D18" s="9">
         <v>100</v>
@@ -3023,9 +2997,11 @@
         <v>87</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="9"/>
+        <v>70</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="H18" s="9"/>
       <c r="I18" s="18"/>
       <c r="J18" s="8">
@@ -3802,18 +3778,18 @@
     <mergeCell ref="A15:A16"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F40">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Aborted">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Aborted">
       <formula>NOT(ISERROR(SEARCH("Aborted",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
MàJ UserStories & Function "updateUser".
</commit_message>
<xml_diff>
--- a/UserStory.xlsx
+++ b/UserStory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="91">
   <si>
     <t>User Story</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>Closed</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Estimated Time</t>
@@ -758,39 +755,39 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1196,56 +1193,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="35"/>
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="38"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:12" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1432,7 +1429,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="30" t="s">
@@ -2158,6 +2155,63 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="73">
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D5:E5"/>
@@ -2174,63 +2228,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2242,7 +2239,7 @@
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2306,10 +2303,10 @@
         <v>60</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>61</v>
@@ -2318,13 +2315,13 @@
         <v>62</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>65</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>66</v>
       </c>
       <c r="J3" s="16">
         <v>42410</v>
@@ -2362,13 +2359,13 @@
         <v>2100</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="17"/>
@@ -2406,13 +2403,13 @@
         <v>1300</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="18"/>
@@ -2450,13 +2447,13 @@
         <v>100</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="28"/>
@@ -2496,13 +2493,13 @@
         <v>800</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="18"/>
@@ -2542,13 +2539,13 @@
         <v>800</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="18"/>
@@ -2586,13 +2583,13 @@
         <v>100</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="18"/>
@@ -2630,13 +2627,13 @@
         <v>100</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="18"/>
@@ -2676,13 +2673,13 @@
         <v>800</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="28"/>
@@ -2728,7 +2725,7 @@
         <v>63</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="18"/>
@@ -2768,13 +2765,13 @@
         <v>700</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="18"/>
@@ -2812,13 +2809,13 @@
         <v>700</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="18"/>
@@ -2858,13 +2855,13 @@
         <v>800</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="18"/>
@@ -2902,13 +2899,13 @@
         <v>500</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="18"/>
@@ -2948,13 +2945,13 @@
         <v>100</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="18"/>
@@ -2994,13 +2991,13 @@
         <v>100</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="18"/>
@@ -3762,7 +3759,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K44">
         <f>SUM(J42:P42)</f>

</xml_diff>

<commit_message>
Modif de la userstory
</commit_message>
<xml_diff>
--- a/UserStory.xlsx
+++ b/UserStory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>User Story</t>
   </si>
@@ -297,7 +297,10 @@
     <t>Ajout d'un parcours (API)</t>
   </si>
   <si>
-    <t>Open</t>
+    <t>Damiano+Marlon</t>
+  </si>
+  <si>
+    <t>Marlon+Damiano</t>
   </si>
 </sst>
 </file>
@@ -764,6 +767,14 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -788,28 +799,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1202,56 +1205,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:12" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="39"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -2164,6 +2167,63 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="73">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H7:K7"/>
@@ -2180,63 +2240,6 @@
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2247,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,7 +2358,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="42" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="8">
@@ -2401,7 +2404,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="9">
         <v>2</v>
       </c>
@@ -2445,7 +2448,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="9">
         <v>3</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>69</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="18"/>
@@ -2475,7 +2478,7 @@
       <c r="P6" s="21"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="26">
         <v>4</v>
       </c>
@@ -2565,7 +2568,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="40" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="9">
@@ -2611,7 +2614,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="8">
         <v>7</v>
       </c>
@@ -2655,7 +2658,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="9">
         <v>8</v>
       </c>
@@ -2791,7 +2794,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="40" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="9">
@@ -2837,7 +2840,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="9">
         <v>12</v>
       </c>
@@ -2881,7 +2884,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="40" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="8">
@@ -2927,7 +2930,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="9">
         <v>14</v>
       </c>
@@ -2941,7 +2944,7 @@
         <v>84</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>74</v>
@@ -3017,7 +3020,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="40" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="8">
@@ -3033,7 +3036,7 @@
         <v>91</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>87</v>
@@ -3063,7 +3066,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="9">
         <v>17</v>
       </c>
@@ -3077,9 +3080,11 @@
         <v>92</v>
       </c>
       <c r="F20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="18"/>
       <c r="J20" s="8">

</xml_diff>